<commit_message>
Looked at some database work
</commit_message>
<xml_diff>
--- a/databases/#Gaylor/week-6 (File Organisations 1)/remainder.xlsx
+++ b/databases/#Gaylor/week-6 (File Organisations 1)/remainder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkBaber\Documents\GitHub\uniWork\databases\Gaylor\week-6 (File Organisations 1)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\uniWork\databases\#Gaylor\week-6 (File Organisations 1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1605D8CA-699F-4954-A44E-1CC31C36326E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5CCBD9-A82A-43A4-952E-71D2A7AB7C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7440" yWindow="2460" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{63FA4009-30A9-4819-A685-54840BBD1287}"/>
+    <workbookView xWindow="5760" yWindow="2496" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{63FA4009-30A9-4819-A685-54840BBD1287}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Hash Keys</t>
   </si>
@@ -92,6 +94,9 @@
   </si>
   <si>
     <t>2b</t>
+  </si>
+  <si>
+    <t>29*</t>
   </si>
 </sst>
 </file>
@@ -478,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C74527-E526-4BE3-94AA-1755231C2D96}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:Q25"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,7 +537,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="1">
-        <f>MOD(F2,G2)</f>
+        <f t="shared" ref="H2:H9" si="0">MOD(F2,G2)</f>
         <v>1</v>
       </c>
     </row>
@@ -547,7 +552,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D20" si="0">MOD(B3,C3)</f>
+        <f t="shared" ref="D3:D10" si="1">MOD(B3,C3)</f>
         <v>1</v>
       </c>
       <c r="F3" s="1">
@@ -557,7 +562,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="1">
-        <f>MOD(F3,G3)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -572,7 +577,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F4" s="1">
@@ -582,7 +587,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="1">
-        <f>MOD(F4,G4)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -597,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F5" s="1">
@@ -607,7 +612,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="1">
-        <f>MOD(F5,G5)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -622,7 +627,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F6" s="1">
@@ -632,7 +637,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="1">
-        <f>MOD(F6,G6)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -647,7 +652,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F7" s="1">
@@ -657,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="1">
-        <f>MOD(F7,G7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -672,7 +677,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F8" s="1">
@@ -682,7 +687,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="1">
-        <f>MOD(F8,G8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -697,7 +702,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F9" s="1">
@@ -707,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="H9" s="1">
-        <f>MOD(F9,G9)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -722,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -794,7 +799,9 @@
       <c r="P15" s="2">
         <v>67</v>
       </c>
-      <c r="Q15" s="2"/>
+      <c r="Q15" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
@@ -823,7 +830,9 @@
       <c r="P16" s="2">
         <v>45</v>
       </c>
-      <c r="Q16" s="2"/>
+      <c r="Q16" s="2">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
@@ -847,7 +856,9 @@
       <c r="P17" s="2">
         <v>27</v>
       </c>
-      <c r="Q17" s="2"/>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
@@ -871,7 +882,9 @@
       <c r="P18" s="2">
         <v>88</v>
       </c>
-      <c r="Q18" s="2"/>
+      <c r="Q18" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
@@ -1012,9 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1F9E3F-C17A-4483-B6BA-A3F0AB004C54}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1032,6 +1043,10 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -1047,6 +1062,9 @@
         <f>MOD(B2,C2)</f>
         <v>1</v>
       </c>
+      <c r="J2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -1062,6 +1080,9 @@
         <f t="shared" ref="D3:D10" si="0">MOD(B3,C3)</f>
         <v>1</v>
       </c>
+      <c r="J3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -1077,6 +1098,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -1092,6 +1116,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1107,6 +1134,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -1122,6 +1152,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -1137,6 +1170,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="J8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1152,6 +1188,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="J9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1167,6 +1206,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="J10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -1322,7 +1364,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="1"/>
       <c r="H16" s="2">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="J16" s="2">
         <v>3</v>
@@ -1331,10 +1373,10 @@
       <c r="L16" s="2"/>
       <c r="M16" s="1"/>
       <c r="N16" s="2">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="O16" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -1350,15 +1392,21 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="2">
+        <v>93</v>
+      </c>
       <c r="J17" s="2">
         <v>4</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="2"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="N17" s="2">
+        <v>93</v>
+      </c>
+      <c r="O17" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
@@ -1416,13 +1464,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="3">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E20" s="2">
         <v>7</v>
       </c>
       <c r="F20" s="3">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1430,7 +1478,7 @@
         <v>7</v>
       </c>
       <c r="K20" s="3">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="1"/>
@@ -1442,7 +1490,9 @@
       <c r="B21" s="2">
         <v>8</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="E21" s="2">
         <v>8</v>
       </c>
@@ -1484,23 +1534,17 @@
       <c r="B23" s="2">
         <v>10</v>
       </c>
-      <c r="C23" s="2">
-        <v>54</v>
-      </c>
+      <c r="C23" s="2"/>
       <c r="E23" s="2">
         <v>10</v>
       </c>
-      <c r="F23" s="2">
-        <v>54</v>
-      </c>
+      <c r="F23" s="2"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="J23" s="2">
         <v>10</v>
       </c>
-      <c r="K23" s="2">
-        <v>54</v>
-      </c>
+      <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>

</xml_diff>